<commit_message>
Updates for new episodes
</commit_message>
<xml_diff>
--- a/webtool/data/money_clean.xlsx
+++ b/webtool/data/money_clean.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trenthenderson/Documents/R/crit-role-webtool/webtool/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trenthenderson/Documents/Git/crit-role-webtool/webtool/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5662CFB4-A949-7A49-BEE7-DE14323FBEB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1200" windowWidth="28160" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>Gained Platinum</t>
   </si>
@@ -394,16 +395,34 @@
     <t>C2E106</t>
   </si>
   <si>
-    <t>TOTALS</t>
-  </si>
-  <si>
     <t>episode</t>
+  </si>
+  <si>
+    <t>C2E107</t>
+  </si>
+  <si>
+    <t>C2E108</t>
+  </si>
+  <si>
+    <t>C2E109</t>
+  </si>
+  <si>
+    <t>C2E110</t>
+  </si>
+  <si>
+    <t>C2E111</t>
+  </si>
+  <si>
+    <t>C2E112</t>
+  </si>
+  <si>
+    <t>C2E113</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -461,6 +480,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -728,18 +750,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="Q104" sqref="Q104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -6087,54 +6109,354 @@
         <v>33766.61</v>
       </c>
     </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>122</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <v>1134</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>1134</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>-4334</v>
+      </c>
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>-4334</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108">
+        <v>-3200</v>
+      </c>
+      <c r="N108">
+        <v>0</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
+      </c>
+      <c r="P108">
+        <v>-3200</v>
+      </c>
+    </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B109">
-        <v>5711</v>
+        <v>0</v>
       </c>
       <c r="C109">
-        <v>89270</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>11607</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>147558.19999999998</v>
+        <v>0</v>
       </c>
       <c r="G109">
-        <v>-1871</v>
+        <v>0</v>
       </c>
       <c r="H109">
-        <v>-81007</v>
+        <v>-50</v>
       </c>
       <c r="I109">
-        <v>-5421</v>
+        <v>0</v>
       </c>
       <c r="J109">
-        <v>-1036</v>
+        <v>0</v>
       </c>
       <c r="K109">
-        <v>-100269.45999999999</v>
+        <v>-50</v>
       </c>
       <c r="L109">
-        <v>3840</v>
+        <v>0</v>
       </c>
       <c r="M109">
-        <v>8263</v>
+        <v>-50</v>
       </c>
       <c r="N109">
-        <v>6186</v>
+        <v>0</v>
       </c>
       <c r="O109">
-        <v>714</v>
+        <v>0</v>
       </c>
       <c r="P109">
-        <v>47288.74</v>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>124</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+      <c r="C110">
+        <v>2400</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>2400</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>-16162</v>
+      </c>
+      <c r="I110">
+        <v>-19</v>
+      </c>
+      <c r="J110">
+        <v>-6</v>
+      </c>
+      <c r="K110">
+        <v>-16163.96</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110">
+        <v>-13762</v>
+      </c>
+      <c r="N110">
+        <v>-19</v>
+      </c>
+      <c r="O110">
+        <v>-6</v>
+      </c>
+      <c r="P110">
+        <v>-13763.96</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>125</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>-420</v>
+      </c>
+      <c r="I111">
+        <v>-3</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <v>-420.3</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111">
+        <v>-420</v>
+      </c>
+      <c r="N111">
+        <v>-3</v>
+      </c>
+      <c r="O111">
+        <v>0</v>
+      </c>
+      <c r="P111">
+        <v>-420.3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>126</v>
+      </c>
+      <c r="B112">
+        <v>546</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>5460</v>
+      </c>
+      <c r="G112">
+        <v>-548</v>
+      </c>
+      <c r="H112">
+        <v>-9961</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+      <c r="K112">
+        <v>-15441</v>
+      </c>
+      <c r="L112">
+        <v>-2</v>
+      </c>
+      <c r="M112">
+        <v>-9961</v>
+      </c>
+      <c r="N112">
+        <v>0</v>
+      </c>
+      <c r="O112">
+        <v>0</v>
+      </c>
+      <c r="P112">
+        <v>-9981</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>127</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>-607</v>
+      </c>
+      <c r="I113">
+        <v>-37</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+      <c r="K113">
+        <v>-610.70000000000005</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113">
+        <v>-607</v>
+      </c>
+      <c r="N113">
+        <v>-37</v>
+      </c>
+      <c r="O113">
+        <v>0</v>
+      </c>
+      <c r="P113">
+        <v>-610.70000000000005</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>128</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <v>0</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+      <c r="N114">
+        <v>0</v>
+      </c>
+      <c r="O114">
+        <v>0</v>
+      </c>
+      <c r="P114">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>